<commit_message>
[PT-BR]Resolvido requisito 1. [EN] Solved 1st requirement
</commit_message>
<xml_diff>
--- a/SpotifyClone-Non-NormalizedTable.xlsx
+++ b/SpotifyClone-Non-NormalizedTable.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
   <si>
     <t xml:space="preserve">albums</t>
   </si>
@@ -73,7 +73,7 @@
     <t xml:space="preserve">Thati</t>
   </si>
   <si>
-    <t xml:space="preserve">0</t>
+    <t xml:space="preserve">1</t>
   </si>
   <si>
     <t xml:space="preserve">gratuito</t>
@@ -85,24 +85,30 @@
     <t xml:space="preserve">Cintia</t>
   </si>
   <si>
-    <t xml:space="preserve">1</t>
+    <t xml:space="preserve">2</t>
   </si>
   <si>
     <t xml:space="preserve">familiar</t>
   </si>
   <si>
+    <t xml:space="preserve">7.99</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hallowed Steam</t>
   </si>
   <si>
     <t xml:space="preserve">Bill</t>
   </si>
   <si>
-    <t xml:space="preserve">2</t>
+    <t xml:space="preserve">3</t>
   </si>
   <si>
     <t xml:space="preserve">universitário</t>
   </si>
   <si>
+    <t xml:space="preserve">5.99</t>
+  </si>
+  <si>
     <t xml:space="preserve">Incandescent</t>
   </si>
   <si>
@@ -167,9 +173,6 @@
   </si>
   <si>
     <t xml:space="preserve">Sweetie, Let's Go Wild</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3</t>
   </si>
   <si>
     <t xml:space="preserve">She Knows</t>
@@ -468,10 +471,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:R36"/>
+  <dimension ref="B1:S36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K16" activeCellId="0" sqref="K16"/>
+      <selection pane="topLeft" activeCell="Q13" activeCellId="0" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -479,7 +482,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.47"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="2.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="2.02"/>
@@ -573,11 +576,19 @@
       <c r="C4" s="10" t="s">
         <v>15</v>
       </c>
+      <c r="D4" s="0" t="str">
+        <f aca="false">CONCATENATE("('",C4,"'),")</f>
+        <v>('Envious'),</v>
+      </c>
       <c r="E4" s="9" t="n">
         <v>1</v>
       </c>
       <c r="F4" s="11" t="n">
         <v>1</v>
+      </c>
+      <c r="G4" s="0" t="str">
+        <f aca="false">CONCATENATE("(",F4,",",E4,"),")</f>
+        <v>(1,1),</v>
       </c>
       <c r="H4" s="9" t="n">
         <v>1</v>
@@ -589,7 +600,11 @@
         <v>23</v>
       </c>
       <c r="K4" s="11" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="L4" s="0" t="str">
+        <f aca="false">CONCATENATE("('",I4,"',",J4,",",K4,"),")</f>
+        <v>('Thati',23,1),</v>
       </c>
       <c r="M4" s="12" t="s">
         <v>17</v>
@@ -600,11 +615,19 @@
       <c r="O4" s="13" t="n">
         <v>0</v>
       </c>
+      <c r="P4" s="0" t="str">
+        <f aca="false">CONCATENATE("('",N4,"',",O4,"),")</f>
+        <v>('gratuito',0),</v>
+      </c>
       <c r="Q4" s="14" t="n">
         <v>1</v>
       </c>
       <c r="R4" s="11" t="n">
         <v>1</v>
+      </c>
+      <c r="S4" s="0" t="str">
+        <f aca="false">CONCATENATE("(",Q4,",",R4,"),")</f>
+        <v>(1,1),</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -614,11 +637,19 @@
       <c r="C5" s="10" t="s">
         <v>19</v>
       </c>
+      <c r="D5" s="0" t="str">
+        <f aca="false">CONCATENATE("('",C5,"'),")</f>
+        <v>('Exuberant'),</v>
+      </c>
       <c r="E5" s="9" t="n">
         <v>1</v>
       </c>
       <c r="F5" s="11" t="n">
         <v>2</v>
+      </c>
+      <c r="G5" s="0" t="str">
+        <f aca="false">CONCATENATE("(",F5,",",E5,"),")</f>
+        <v>(2,1),</v>
       </c>
       <c r="H5" s="9" t="n">
         <v>2</v>
@@ -630,7 +661,11 @@
         <v>35</v>
       </c>
       <c r="K5" s="11" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="L5" s="0" t="str">
+        <f aca="false">CONCATENATE("('",I5,"',",J5,",",K5,"),")</f>
+        <v>('Cintia',35,2),</v>
       </c>
       <c r="M5" s="12" t="s">
         <v>21</v>
@@ -638,14 +673,22 @@
       <c r="N5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="13" t="n">
-        <v>7.99</v>
+      <c r="O5" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="P5" s="0" t="str">
+        <f aca="false">CONCATENATE("('",N5,"',",O5,"),")</f>
+        <v>('familiar',7.99),</v>
       </c>
       <c r="Q5" s="11" t="n">
         <v>1</v>
       </c>
       <c r="R5" s="11" t="n">
         <v>4</v>
+      </c>
+      <c r="S5" s="0" t="str">
+        <f aca="false">CONCATENATE("(",Q5,",",R5,"),")</f>
+        <v>(1,4),</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -653,7 +696,11 @@
         <v>3</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="D6" s="0" t="str">
+        <f aca="false">CONCATENATE("('",C6,"'),")</f>
+        <v>('Hallowed Steam'),</v>
       </c>
       <c r="E6" s="9" t="n">
         <v>1</v>
@@ -661,32 +708,48 @@
       <c r="F6" s="11" t="n">
         <v>3</v>
       </c>
+      <c r="G6" s="0" t="str">
+        <f aca="false">CONCATENATE("(",F6,",",E6,"),")</f>
+        <v>(3,1),</v>
+      </c>
       <c r="H6" s="9" t="n">
         <v>3</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J6" s="9" t="n">
         <v>20</v>
       </c>
       <c r="K6" s="11" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="L6" s="0" t="str">
+        <f aca="false">CONCATENATE("('",I6,"',",J6,",",K6,"),")</f>
+        <v>('Bill',20,3),</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N6" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="O6" s="13" t="n">
-        <v>5.99</v>
+        <v>27</v>
+      </c>
+      <c r="O6" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="P6" s="0" t="str">
+        <f aca="false">CONCATENATE("('",N6,"',",O6,"),")</f>
+        <v>('universitário',5.99),</v>
       </c>
       <c r="Q6" s="11" t="n">
         <v>1</v>
       </c>
       <c r="R6" s="11" t="n">
         <v>3</v>
+      </c>
+      <c r="S6" s="0" t="str">
+        <f aca="false">CONCATENATE("(",Q6,",",R6,"),")</f>
+        <v>(1,3),</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -694,7 +757,11 @@
         <v>4</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="D7" s="0" t="str">
+        <f aca="false">CONCATENATE("('",C7,"'),")</f>
+        <v>('Incandescent'),</v>
       </c>
       <c r="E7" s="9" t="n">
         <v>2</v>
@@ -702,23 +769,35 @@
       <c r="F7" s="11" t="n">
         <v>4</v>
       </c>
+      <c r="G7" s="0" t="str">
+        <f aca="false">CONCATENATE("(",F7,",",E7,"),")</f>
+        <v>(4,2),</v>
+      </c>
       <c r="H7" s="9" t="n">
         <v>4</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J7" s="9" t="n">
         <v>45</v>
       </c>
       <c r="K7" s="11" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="L7" s="0" t="str">
+        <f aca="false">CONCATENATE("('",I7,"',",J7,",",K7,"),")</f>
+        <v>('Roger',45,1),</v>
       </c>
       <c r="Q7" s="11" t="n">
         <v>2</v>
       </c>
       <c r="R7" s="11" t="n">
         <v>1</v>
+      </c>
+      <c r="S7" s="0" t="str">
+        <f aca="false">CONCATENATE("(",Q7,",",R7,"),")</f>
+        <v>(2,1),</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -726,7 +805,11 @@
         <v>5</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+      <c r="D8" s="0" t="str">
+        <f aca="false">CONCATENATE("('",C8,"'),")</f>
+        <v>('Temporary Culture'),</v>
       </c>
       <c r="E8" s="9" t="n">
         <v>2</v>
@@ -734,11 +817,19 @@
       <c r="F8" s="11" t="n">
         <v>5</v>
       </c>
+      <c r="G8" s="0" t="str">
+        <f aca="false">CONCATENATE("(",F8,",",E8,"),")</f>
+        <v>(5,2),</v>
+      </c>
       <c r="Q8" s="11" t="n">
         <v>2</v>
       </c>
       <c r="R8" s="11" t="n">
         <v>3</v>
+      </c>
+      <c r="S8" s="0" t="str">
+        <f aca="false">CONCATENATE("(",Q8,",",R8,"),")</f>
+        <v>(2,3),</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -748,16 +839,24 @@
       <c r="F9" s="11" t="n">
         <v>6</v>
       </c>
+      <c r="G9" s="0" t="str">
+        <f aca="false">CONCATENATE("(",F9,",",E9,"),")</f>
+        <v>(6,3),</v>
+      </c>
       <c r="Q9" s="11" t="n">
         <v>3</v>
       </c>
       <c r="R9" s="11" t="n">
         <v>2</v>
+      </c>
+      <c r="S9" s="0" t="str">
+        <f aca="false">CONCATENATE("(",Q9,",",R9,"),")</f>
+        <v>(3,2),</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C10" s="5"/>
       <c r="E10" s="11" t="n">
@@ -766,11 +865,19 @@
       <c r="F10" s="11" t="n">
         <v>7</v>
       </c>
+      <c r="G10" s="0" t="str">
+        <f aca="false">CONCATENATE("(",F10,",",E10,"),")</f>
+        <v>(7,3),</v>
+      </c>
       <c r="Q10" s="11" t="n">
         <v>3</v>
       </c>
       <c r="R10" s="11" t="n">
         <v>1</v>
+      </c>
+      <c r="S10" s="0" t="str">
+        <f aca="false">CONCATENATE("(",Q10,",",R10,"),")</f>
+        <v>(3,1),</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -778,7 +885,7 @@
         <v>14</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E11" s="11" t="n">
         <v>3</v>
@@ -786,11 +893,19 @@
       <c r="F11" s="11" t="n">
         <v>8</v>
       </c>
+      <c r="G11" s="0" t="str">
+        <f aca="false">CONCATENATE("(",F11,",",E11,"),")</f>
+        <v>(8,3),</v>
+      </c>
       <c r="Q11" s="11" t="n">
         <v>4</v>
       </c>
       <c r="R11" s="11" t="n">
         <v>4</v>
+      </c>
+      <c r="S11" s="0" t="str">
+        <f aca="false">CONCATENATE("(",Q11,",",R11,"),")</f>
+        <v>(4,4),</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -798,7 +913,11 @@
         <v>1</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="D12" s="0" t="str">
+        <f aca="false">CONCATENATE("('",C12,"'),")</f>
+        <v>('Walter Phoenix'),</v>
       </c>
       <c r="E12" s="11" t="n">
         <v>3</v>
@@ -806,13 +925,21 @@
       <c r="F12" s="11" t="n">
         <v>9</v>
       </c>
+      <c r="G12" s="0" t="str">
+        <f aca="false">CONCATENATE("(",F12,",",E12,"),")</f>
+        <v>(9,3),</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="11" t="n">
         <v>2</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="D13" s="0" t="str">
+        <f aca="false">CONCATENATE("('",C13,"'),")</f>
+        <v>('Peter Strong'),</v>
       </c>
       <c r="E13" s="11" t="n">
         <v>4</v>
@@ -820,8 +947,12 @@
       <c r="F13" s="11" t="n">
         <v>10</v>
       </c>
+      <c r="G13" s="0" t="str">
+        <f aca="false">CONCATENATE("(",F13,",",E13,"),")</f>
+        <v>(10,4),</v>
+      </c>
       <c r="Q13" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="R13" s="5"/>
     </row>
@@ -830,7 +961,11 @@
         <v>3</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>35</v>
+        <v>37</v>
+      </c>
+      <c r="D14" s="0" t="str">
+        <f aca="false">CONCATENATE("('",C14,"'),")</f>
+        <v>('Lance Day'),</v>
       </c>
       <c r="E14" s="11" t="n">
         <v>4</v>
@@ -838,6 +973,10 @@
       <c r="F14" s="11" t="n">
         <v>11</v>
       </c>
+      <c r="G14" s="0" t="str">
+        <f aca="false">CONCATENATE("(",F14,",",E14,"),")</f>
+        <v>(11,4),</v>
+      </c>
       <c r="Q14" s="8" t="s">
         <v>8</v>
       </c>
@@ -850,7 +989,11 @@
         <v>4</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="D15" s="0" t="str">
+        <f aca="false">CONCATENATE("('",C15,"'),")</f>
+        <v>('Freedie Shannon'),</v>
       </c>
       <c r="E15" s="11" t="n">
         <v>4</v>
@@ -858,11 +1001,19 @@
       <c r="F15" s="11" t="n">
         <v>12</v>
       </c>
+      <c r="G15" s="0" t="str">
+        <f aca="false">CONCATENATE("(",F15,",",E15,"),")</f>
+        <v>(12,4),</v>
+      </c>
       <c r="Q15" s="14" t="n">
         <v>1</v>
       </c>
       <c r="R15" s="17" t="n">
         <v>1</v>
+      </c>
+      <c r="S15" s="0" t="str">
+        <f aca="false">CONCATENATE("(",Q15,",",R15,"),")</f>
+        <v>(1,1),</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -872,16 +1023,24 @@
       <c r="F16" s="11" t="n">
         <v>13</v>
       </c>
+      <c r="G16" s="0" t="str">
+        <f aca="false">CONCATENATE("(",F16,",",E16,"),")</f>
+        <v>(13,4),</v>
+      </c>
       <c r="Q16" s="11" t="n">
         <v>1</v>
       </c>
       <c r="R16" s="17" t="n">
         <v>6</v>
       </c>
+      <c r="S16" s="0" t="str">
+        <f aca="false">CONCATENATE("(",Q16,",",R16,"),")</f>
+        <v>(1,6),</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C17" s="5"/>
       <c r="E17" s="11" t="n">
@@ -890,11 +1049,19 @@
       <c r="F17" s="11" t="n">
         <v>14</v>
       </c>
+      <c r="G17" s="0" t="str">
+        <f aca="false">CONCATENATE("(",F17,",",E17,"),")</f>
+        <v>(14,4),</v>
+      </c>
       <c r="Q17" s="11" t="n">
         <v>1</v>
       </c>
       <c r="R17" s="17" t="n">
         <v>14</v>
+      </c>
+      <c r="S17" s="0" t="str">
+        <f aca="false">CONCATENATE("(",Q17,",",R17,"),")</f>
+        <v>(1,14),</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -902,7 +1069,7 @@
         <v>7</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E18" s="11" t="n">
         <v>4</v>
@@ -910,19 +1077,31 @@
       <c r="F18" s="11" t="n">
         <v>15</v>
       </c>
+      <c r="G18" s="0" t="str">
+        <f aca="false">CONCATENATE("(",F18,",",E18,"),")</f>
+        <v>(15,4),</v>
+      </c>
       <c r="Q18" s="11" t="n">
         <v>1</v>
       </c>
       <c r="R18" s="17" t="n">
         <v>16</v>
       </c>
+      <c r="S18" s="0" t="str">
+        <f aca="false">CONCATENATE("(",Q18,",",R18,"),")</f>
+        <v>(1,16),</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="11" t="n">
         <v>1</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>39</v>
+        <v>41</v>
+      </c>
+      <c r="D19" s="0" t="str">
+        <f aca="false">CONCATENATE("('",C19,"'),")</f>
+        <v>('Soul For Us'),</v>
       </c>
       <c r="E19" s="11" t="n">
         <v>5</v>
@@ -930,11 +1109,19 @@
       <c r="F19" s="11" t="n">
         <v>16</v>
       </c>
+      <c r="G19" s="0" t="str">
+        <f aca="false">CONCATENATE("(",F19,",",E19,"),")</f>
+        <v>(16,5),</v>
+      </c>
       <c r="Q19" s="11" t="n">
         <v>2</v>
       </c>
       <c r="R19" s="19" t="s">
-        <v>40</v>
+        <v>42</v>
+      </c>
+      <c r="S19" s="0" t="str">
+        <f aca="false">CONCATENATE("(",Q19,",",R19,"),")</f>
+        <v>(2,13),</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -942,7 +1129,11 @@
         <v>2</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>41</v>
+        <v>43</v>
+      </c>
+      <c r="D20" s="0" t="str">
+        <f aca="false">CONCATENATE("('",C20,"'),")</f>
+        <v>('Reflections Of Magic'),</v>
       </c>
       <c r="E20" s="11" t="n">
         <v>5</v>
@@ -950,19 +1141,31 @@
       <c r="F20" s="11" t="n">
         <v>17</v>
       </c>
+      <c r="G20" s="0" t="str">
+        <f aca="false">CONCATENATE("(",F20,",",E20,"),")</f>
+        <v>(17,5),</v>
+      </c>
       <c r="Q20" s="11" t="n">
         <v>2</v>
       </c>
       <c r="R20" s="17" t="n">
         <v>17</v>
       </c>
+      <c r="S20" s="0" t="str">
+        <f aca="false">CONCATENATE("(",Q20,",",R20,"),")</f>
+        <v>(2,17),</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="11" t="n">
         <v>3</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="D21" s="0" t="str">
+        <f aca="false">CONCATENATE("('",C21,"'),")</f>
+        <v>('Dance With Her Own'),</v>
       </c>
       <c r="E21" s="11" t="n">
         <v>5</v>
@@ -970,11 +1173,19 @@
       <c r="F21" s="11" t="n">
         <v>18</v>
       </c>
+      <c r="G21" s="0" t="str">
+        <f aca="false">CONCATENATE("(",F21,",",E21,"),")</f>
+        <v>(18,5),</v>
+      </c>
       <c r="Q21" s="11" t="n">
         <v>2</v>
       </c>
       <c r="R21" s="17" t="n">
         <v>2</v>
+      </c>
+      <c r="S21" s="0" t="str">
+        <f aca="false">CONCATENATE("(",Q21,",",R21,"),")</f>
+        <v>(2,2),</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -982,13 +1193,21 @@
         <v>4</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>43</v>
+        <v>45</v>
+      </c>
+      <c r="D22" s="0" t="str">
+        <f aca="false">CONCATENATE("('",C22,"'),")</f>
+        <v>('Troubles Of My Inner Fire'),</v>
       </c>
       <c r="Q22" s="11" t="n">
         <v>2</v>
       </c>
       <c r="R22" s="17" t="n">
         <v>15</v>
+      </c>
+      <c r="S22" s="0" t="str">
+        <f aca="false">CONCATENATE("(",Q22,",",R22,"),")</f>
+        <v>(2,15),</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -996,14 +1215,22 @@
         <v>5</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>44</v>
+        <v>46</v>
+      </c>
+      <c r="D23" s="0" t="str">
+        <f aca="false">CONCATENATE("('",C23,"'),")</f>
+        <v>('Time Fireworks'),</v>
       </c>
       <c r="E23" s="20"/>
       <c r="Q23" s="11" t="n">
         <v>3</v>
       </c>
       <c r="R23" s="19" t="s">
-        <v>45</v>
+        <v>47</v>
+      </c>
+      <c r="S23" s="0" t="str">
+        <f aca="false">CONCATENATE("(",Q23,",",R23,"),")</f>
+        <v>(3,4),</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1011,13 +1238,21 @@
         <v>6</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>46</v>
+        <v>48</v>
+      </c>
+      <c r="D24" s="0" t="str">
+        <f aca="false">CONCATENATE("('",C24,"'),")</f>
+        <v>('Magic Circus'),</v>
       </c>
       <c r="Q24" s="11" t="n">
         <v>3</v>
       </c>
       <c r="R24" s="17" t="n">
         <v>16</v>
+      </c>
+      <c r="S24" s="0" t="str">
+        <f aca="false">CONCATENATE("(",Q24,",",R24,"),")</f>
+        <v>(3,16),</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1025,13 +1260,21 @@
         <v>7</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>47</v>
+        <v>49</v>
+      </c>
+      <c r="D25" s="0" t="str">
+        <f aca="false">CONCATENATE("('",C25,"'),")</f>
+        <v>('Honey, So Do I'),</v>
       </c>
       <c r="Q25" s="11" t="n">
         <v>3</v>
       </c>
       <c r="R25" s="17" t="n">
         <v>6</v>
+      </c>
+      <c r="S25" s="0" t="str">
+        <f aca="false">CONCATENATE("(",Q25,",",R25,"),")</f>
+        <v>(3,6),</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1039,13 +1282,21 @@
         <v>8</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>48</v>
+        <v>50</v>
+      </c>
+      <c r="D26" s="0" t="str">
+        <f aca="false">CONCATENATE("('",C26,"'),")</f>
+        <v>('Sweetie, Let's Go Wild'),</v>
       </c>
       <c r="Q26" s="11" t="n">
         <v>4</v>
       </c>
       <c r="R26" s="19" t="s">
-        <v>49</v>
+        <v>26</v>
+      </c>
+      <c r="S26" s="0" t="str">
+        <f aca="false">CONCATENATE("(",Q26,",",R26,"),")</f>
+        <v>(4,3),</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1053,13 +1304,21 @@
         <v>9</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="D27" s="0" t="str">
+        <f aca="false">CONCATENATE("('",C27,"'),")</f>
+        <v>('She Knows'),</v>
       </c>
       <c r="Q27" s="11" t="n">
         <v>4</v>
       </c>
       <c r="R27" s="17" t="n">
         <v>18</v>
+      </c>
+      <c r="S27" s="0" t="str">
+        <f aca="false">CONCATENATE("(",Q27,",",R27,"),")</f>
+        <v>(4,18),</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1067,13 +1326,21 @@
         <v>10</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>51</v>
+        <v>52</v>
+      </c>
+      <c r="D28" s="0" t="str">
+        <f aca="false">CONCATENATE("('",C28,"'),")</f>
+        <v>('Fantasy For Me'),</v>
       </c>
       <c r="Q28" s="11" t="n">
         <v>4</v>
       </c>
       <c r="R28" s="17" t="n">
         <v>11</v>
+      </c>
+      <c r="S28" s="0" t="str">
+        <f aca="false">CONCATENATE("(",Q28,",",R28,"),")</f>
+        <v>(4,11),</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1081,7 +1348,11 @@
         <v>11</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+      <c r="D29" s="0" t="str">
+        <f aca="false">CONCATENATE("('",C29,"'),")</f>
+        <v>('Celebration Of More'),</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1089,7 +1360,11 @@
         <v>12</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="D30" s="0" t="str">
+        <f aca="false">CONCATENATE("('",C30,"'),")</f>
+        <v>('Rock His Everything'),</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1097,7 +1372,11 @@
         <v>13</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>54</v>
+        <v>55</v>
+      </c>
+      <c r="D31" s="0" t="str">
+        <f aca="false">CONCATENATE("('",C31,"'),")</f>
+        <v>('Home Forever'),</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1105,7 +1384,11 @@
         <v>14</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+      <c r="D32" s="0" t="str">
+        <f aca="false">CONCATENATE("('",C32,"'),")</f>
+        <v>('Diamond Power'),</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1113,7 +1396,11 @@
         <v>15</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+      <c r="D33" s="0" t="str">
+        <f aca="false">CONCATENATE("('",C33,"'),")</f>
+        <v>('Honey, Let's Be Silly'),</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1121,7 +1408,11 @@
         <v>16</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="D34" s="0" t="str">
+        <f aca="false">CONCATENATE("('",C34,"'),")</f>
+        <v>('Thang Of Thunder'),</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1129,7 +1420,11 @@
         <v>17</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>58</v>
+        <v>59</v>
+      </c>
+      <c r="D35" s="0" t="str">
+        <f aca="false">CONCATENATE("('",C35,"'),")</f>
+        <v>('Words Of Her Life'),</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1137,7 +1432,11 @@
         <v>18</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>59</v>
+        <v>60</v>
+      </c>
+      <c r="D36" s="0" t="str">
+        <f aca="false">CONCATENATE("('",C36,"'),")</f>
+        <v>('Without My Streets'),</v>
       </c>
     </row>
   </sheetData>

</xml_diff>